<commit_message>
+1.5 page of text/result/etc added
+ some data transform magic in excel
</commit_message>
<xml_diff>
--- a/SearchAndHyperlinking/results/allresult.xlsx
+++ b/SearchAndHyperlinking/results/allresult.xlsx
@@ -9,22 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24315" windowHeight="10800" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24315" windowHeight="10800" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="search P_5" sheetId="1" r:id="rId1"/>
     <sheet name="search P_10" sheetId="2" r:id="rId2"/>
-    <sheet name="search P_20" sheetId="3" r:id="rId3"/>
-    <sheet name="link P_5" sheetId="4" r:id="rId4"/>
-    <sheet name="link P_10" sheetId="5" r:id="rId5"/>
-    <sheet name="link P_20" sheetId="6" r:id="rId6"/>
+    <sheet name="Munka1" sheetId="7" r:id="rId3"/>
+    <sheet name="search P_20" sheetId="3" r:id="rId4"/>
+    <sheet name="link P_5" sheetId="4" r:id="rId5"/>
+    <sheet name="link P_10" sheetId="5" r:id="rId6"/>
+    <sheet name="link P_20" sheetId="6" r:id="rId7"/>
+    <sheet name="search P_10 stat" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -738,6 +740,2026 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'search P_10 stat'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manual subtitles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:tint val="88500"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="88500"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$14:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>7.7777777777777779E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.666666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25555555555555559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61111111111111116</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27777777777777785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$2:$AA$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'search P_10 stat'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LIMSI transcripts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:tint val="55000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="55000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$14:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>7.7777777777777779E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.666666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25555555555555559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61111111111111116</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27777777777777785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$3:$AA$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'search P_10 stat'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LIUM transcripts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:tint val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$14:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>7.7777777777777779E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.666666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25555555555555559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61111111111111116</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27777777777777785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$4:$AA$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'search P_10 stat'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NST/Sheffield</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="98500"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$14:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>7.7777777777777779E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.666666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25555555555555559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61111111111111116</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27777777777777785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$5:$AA$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'search P_10 stat'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All transcript and subtitle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="30000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$14:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>7.7777777777777779E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.666666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25555555555555559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.61111111111111116</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.18888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.27777777777777785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'search P_10 stat'!$B$6:$AA$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="299218688"/>
+        <c:axId val="299211968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="299218688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299211968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="299211968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299218688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Táblázat2" displayName="Táblázat2" ref="A1:AA14" totalsRowShown="0">
+  <autoFilter ref="A1:AA14"/>
+  <tableColumns count="27">
+    <tableColumn id="1" name="name"/>
+    <tableColumn id="3" name="query_11"/>
+    <tableColumn id="4" name="query_12"/>
+    <tableColumn id="5" name="query_13"/>
+    <tableColumn id="6" name="query_14"/>
+    <tableColumn id="7" name="query_15"/>
+    <tableColumn id="8" name="query_17"/>
+    <tableColumn id="9" name="query_18"/>
+    <tableColumn id="10" name="query_19"/>
+    <tableColumn id="11" name="query_2"/>
+    <tableColumn id="12" name="query_20"/>
+    <tableColumn id="13" name="query_21"/>
+    <tableColumn id="14" name="query_26"/>
+    <tableColumn id="15" name="query_27"/>
+    <tableColumn id="16" name="query_28"/>
+    <tableColumn id="17" name="query_29"/>
+    <tableColumn id="18" name="query_30"/>
+    <tableColumn id="19" name="query_31"/>
+    <tableColumn id="20" name="query_32"/>
+    <tableColumn id="21" name="query_33"/>
+    <tableColumn id="22" name="query_34"/>
+    <tableColumn id="23" name="query_35"/>
+    <tableColumn id="24" name="query_36"/>
+    <tableColumn id="25" name="query_4"/>
+    <tableColumn id="26" name="query_5"/>
+    <tableColumn id="27" name="query_7"/>
+    <tableColumn id="28" name="query_9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
@@ -1003,8 +3025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG16"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH18" sqref="AH18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC13" sqref="A13:AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,10 +4432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3403,6 +5425,123 @@
         <v>0.15859999999999999</v>
       </c>
     </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(B3:B12)</f>
+        <v>0.3</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:AC14" si="0">AVERAGE(C3:C12)</f>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>6.666666666666668E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.18888888888888891</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.25555555555555559</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>0.14444444444444446</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>0.34444444444444444</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="0"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="0"/>
+        <v>0.12222222222222223</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="0"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="0"/>
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="0"/>
+        <v>0.18888888888888891</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="0"/>
+        <v>0.27777777777777785</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="0"/>
+        <v>0.20440000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3410,10 +5549,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,376 +6549,6 @@
       </c>
       <c r="AC11">
         <v>0.11899999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2">
-        <v>0.2</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.4</v>
-      </c>
-      <c r="J2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>4.4400000000000002E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0.4</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>5.33E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0.2</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0.4</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>3.6999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7">
-        <v>0.2</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0.6</v>
-      </c>
-      <c r="J7">
-        <v>0.18179999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>5.2600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0.2</v>
-      </c>
-      <c r="H10">
-        <v>0.2</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0.4</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>1.43E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4780,7 +6561,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4825,7 +6606,7 @@
         <v>29</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4846,10 +6627,10 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="J2">
-        <v>0.05</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4881,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>3.3300000000000003E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -4889,7 +6670,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -4907,13 +6688,13 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.04</v>
+        <v>5.33E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4936,16 +6717,16 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>4.6699999999999998E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4962,7 +6743,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -4977,7 +6758,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>4.07E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4985,7 +6766,7 @@
         <v>34</v>
       </c>
       <c r="B7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -5006,10 +6787,10 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="J7">
-        <v>0.1</v>
+        <v>0.18179999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5041,7 +6822,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>6.25E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5049,7 +6830,7 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -5073,7 +6854,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>3.1600000000000003E-2</v>
+        <v>5.2600000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5087,7 +6868,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -5099,13 +6880,13 @@
         <v>0.2</v>
       </c>
       <c r="H10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -5122,7 +6903,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -5137,7 +6918,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>2.5000000000000001E-2</v>
+        <v>1.43E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5150,7 +6931,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5195,31 +6976,31 @@
         <v>29</v>
       </c>
       <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.3</v>
+      </c>
+      <c r="J2">
         <v>0.05</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.2</v>
-      </c>
-      <c r="J2">
-        <v>3.1199999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5251,7 +7032,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1.67E-2</v>
+        <v>3.3300000000000003E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5259,7 +7040,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5277,13 +7058,13 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5306,16 +7087,16 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>2.3300000000000001E-2</v>
+        <v>4.6699999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -5332,7 +7113,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -5347,7 +7128,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>2.2200000000000001E-2</v>
+        <v>4.07E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5355,7 +7136,7 @@
         <v>34</v>
       </c>
       <c r="B7">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -5376,10 +7157,10 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J7">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5411,7 +7192,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>3.7499999999999999E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5419,13 +7200,13 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -5443,7 +7224,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1.84E-2</v>
+        <v>3.1600000000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5457,7 +7238,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -5466,16 +7247,16 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H10">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1.7500000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -5492,7 +7273,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -5507,10 +7288,1468 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1.9599999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>0.05</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.2</v>
+      </c>
+      <c r="J2">
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1.67E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0.05</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>2.3300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.15</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>2.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.2</v>
+      </c>
+      <c r="J7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>0.05</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.05</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1.84E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0.05</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="23" width="11.140625" customWidth="1"/>
+    <col min="24" max="27" width="10.140625" customWidth="1"/>
+    <col min="28" max="28" width="8.140625" customWidth="1"/>
+    <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.2</v>
+      </c>
+      <c r="J2">
+        <v>0.1</v>
+      </c>
+      <c r="K2">
+        <v>0.2</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0.1</v>
+      </c>
+      <c r="O2">
+        <v>0.2</v>
+      </c>
+      <c r="P2">
+        <v>0.3</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0.2</v>
+      </c>
+      <c r="S2">
+        <v>0.1</v>
+      </c>
+      <c r="T2">
+        <v>0.9</v>
+      </c>
+      <c r="U2">
+        <v>0.2</v>
+      </c>
+      <c r="V2">
+        <v>0.3</v>
+      </c>
+      <c r="W2">
+        <v>0.1</v>
+      </c>
+      <c r="X2">
+        <v>0.1</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AC2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.2</v>
+      </c>
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.4</v>
+      </c>
+      <c r="J3">
+        <v>0.1</v>
+      </c>
+      <c r="K3">
+        <v>0.5</v>
+      </c>
+      <c r="L3">
+        <v>0.2</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0.2</v>
+      </c>
+      <c r="O3">
+        <v>0.1</v>
+      </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+      <c r="Q3">
+        <v>0.1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0.8</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0.1</v>
+      </c>
+      <c r="X3">
+        <v>0.2</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0.2</v>
+      </c>
+      <c r="AA3">
+        <v>0.3</v>
+      </c>
+      <c r="AC3">
+        <v>0.16669999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0.4</v>
+      </c>
+      <c r="L4">
+        <v>0.1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0.1</v>
+      </c>
+      <c r="O4">
+        <v>0.3</v>
+      </c>
+      <c r="P4">
+        <v>0.6</v>
+      </c>
+      <c r="Q4">
+        <v>0.1</v>
+      </c>
+      <c r="R4">
+        <v>0.1</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0.8</v>
+      </c>
+      <c r="U4">
+        <v>0.1</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0.2</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0.1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0.1444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.1</v>
+      </c>
+      <c r="J5">
+        <v>0.1</v>
+      </c>
+      <c r="K5">
+        <v>0.4</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0.2</v>
+      </c>
+      <c r="O5">
+        <v>0.2</v>
+      </c>
+      <c r="P5">
+        <v>0.3</v>
+      </c>
+      <c r="Q5">
+        <v>0.1</v>
+      </c>
+      <c r="R5">
+        <v>0.2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0.1</v>
+      </c>
+      <c r="W5">
+        <v>0.2</v>
+      </c>
+      <c r="X5">
+        <v>0.1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0.2</v>
+      </c>
+      <c r="AA5">
+        <v>0.5</v>
+      </c>
+      <c r="AC5">
+        <v>0.1308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0.3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.4</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.4</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0.2</v>
+      </c>
+      <c r="O6">
+        <v>0.3</v>
+      </c>
+      <c r="P6">
+        <v>0.5</v>
+      </c>
+      <c r="Q6">
+        <v>0.1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0.7</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0.1</v>
+      </c>
+      <c r="AA6">
+        <v>0.2</v>
+      </c>
+      <c r="AC6">
+        <v>0.13450000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>0.2</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>0.3</v>
+      </c>
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+      <c r="I7">
+        <v>0.3</v>
+      </c>
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+      <c r="K7">
+        <v>0.4</v>
+      </c>
+      <c r="L7">
+        <v>0.1</v>
+      </c>
+      <c r="M7">
+        <v>0.2</v>
+      </c>
+      <c r="N7">
+        <v>0.2</v>
+      </c>
+      <c r="O7">
+        <v>0.5</v>
+      </c>
+      <c r="P7">
+        <v>0.6</v>
+      </c>
+      <c r="Q7">
+        <v>0.1</v>
+      </c>
+      <c r="R7">
+        <v>0.3</v>
+      </c>
+      <c r="S7">
+        <v>0.4</v>
+      </c>
+      <c r="T7">
+        <v>0.9</v>
+      </c>
+      <c r="U7">
+        <v>0.2</v>
+      </c>
+      <c r="V7">
+        <v>0.5</v>
+      </c>
+      <c r="W7">
+        <v>0.1</v>
+      </c>
+      <c r="X7">
+        <v>0.3</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0.2</v>
+      </c>
+      <c r="AA7">
+        <v>0.5</v>
+      </c>
+      <c r="AC7">
+        <v>0.30740000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.2</v>
+      </c>
+      <c r="I8">
+        <v>0.3</v>
+      </c>
+      <c r="J8">
+        <v>0.1</v>
+      </c>
+      <c r="K8">
+        <v>0.5</v>
+      </c>
+      <c r="L8">
+        <v>0.1</v>
+      </c>
+      <c r="M8">
+        <v>0.4</v>
+      </c>
+      <c r="N8">
+        <v>0.2</v>
+      </c>
+      <c r="O8">
+        <v>0.2</v>
+      </c>
+      <c r="P8">
+        <v>0.6</v>
+      </c>
+      <c r="Q8">
+        <v>0.2</v>
+      </c>
+      <c r="R8">
+        <v>0.3</v>
+      </c>
+      <c r="S8">
+        <v>0.9</v>
+      </c>
+      <c r="T8">
+        <v>0.7</v>
+      </c>
+      <c r="U8">
+        <v>0.3</v>
+      </c>
+      <c r="V8">
+        <v>0.4</v>
+      </c>
+      <c r="W8">
+        <v>0.1</v>
+      </c>
+      <c r="X8">
+        <v>0.3</v>
+      </c>
+      <c r="Y8">
+        <v>0.1</v>
+      </c>
+      <c r="Z8">
+        <v>0.3</v>
+      </c>
+      <c r="AA8">
+        <v>0.3</v>
+      </c>
+      <c r="AC8">
+        <v>0.29260000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>0.8</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.9</v>
+      </c>
+      <c r="I9">
+        <v>0.3</v>
+      </c>
+      <c r="J9">
+        <v>0.1</v>
+      </c>
+      <c r="K9">
+        <v>0.4</v>
+      </c>
+      <c r="L9">
+        <v>0.1</v>
+      </c>
+      <c r="M9">
+        <v>0.4</v>
+      </c>
+      <c r="N9">
+        <v>0.4</v>
+      </c>
+      <c r="O9">
+        <v>0.2</v>
+      </c>
+      <c r="P9">
+        <v>0.5</v>
+      </c>
+      <c r="Q9">
+        <v>0.1</v>
+      </c>
+      <c r="R9">
+        <v>0.2</v>
+      </c>
+      <c r="S9">
+        <v>0.7</v>
+      </c>
+      <c r="T9">
+        <v>0.9</v>
+      </c>
+      <c r="U9">
+        <v>0.2</v>
+      </c>
+      <c r="V9">
+        <v>0.2</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0.1</v>
+      </c>
+      <c r="Y9">
+        <v>0.1</v>
+      </c>
+      <c r="Z9">
+        <v>0.3</v>
+      </c>
+      <c r="AA9">
+        <v>0.1</v>
+      </c>
+      <c r="AC9">
+        <v>0.28149999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>0.1</v>
+      </c>
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>0.3</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.4</v>
+      </c>
+      <c r="I10">
+        <v>0.3</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0.3</v>
+      </c>
+      <c r="L10">
+        <v>0.2</v>
+      </c>
+      <c r="M10">
+        <v>0.5</v>
+      </c>
+      <c r="N10">
+        <v>0.3</v>
+      </c>
+      <c r="O10">
+        <v>0.3</v>
+      </c>
+      <c r="P10">
+        <v>0.2</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0.2</v>
+      </c>
+      <c r="S10">
+        <v>0.9</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0.2</v>
+      </c>
+      <c r="V10">
+        <v>0.3</v>
+      </c>
+      <c r="W10">
+        <v>0.1</v>
+      </c>
+      <c r="X10">
+        <v>0.3</v>
+      </c>
+      <c r="Y10">
+        <v>0.1</v>
+      </c>
+      <c r="Z10">
+        <v>0.1</v>
+      </c>
+      <c r="AA10">
+        <v>0.4</v>
+      </c>
+      <c r="AC10">
+        <v>0.22309999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0.2</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.4</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.4</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0.2</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0.2</v>
+      </c>
+      <c r="O11">
+        <v>0.3</v>
+      </c>
+      <c r="P11">
+        <v>0.4</v>
+      </c>
+      <c r="Q11">
+        <v>0.1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0.2</v>
+      </c>
+      <c r="T11">
+        <v>0.7</v>
+      </c>
+      <c r="U11">
+        <v>0.1</v>
+      </c>
+      <c r="V11">
+        <v>0.1</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0.2</v>
+      </c>
+      <c r="AA11">
+        <v>0.2</v>
+      </c>
+      <c r="AC11">
+        <v>0.15859999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:AC14" si="0">AVERAGE(B3:B12)</f>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>6.666666666666668E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.18888888888888891</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.25555555555555559</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>0.14444444444444446</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>0.34444444444444444</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="0"/>
+        <v>0.12222222222222223</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="0"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="0"/>
+        <v>0.18888888888888891</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="0"/>
+        <v>0.27777777777777785</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="0"/>
+        <v>0.20440000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>